<commit_message>
Upload Input.xlsx via GitHub Pages
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -582,7 +582,7 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>John Deery</t>
+          <t>Branan Harrison</t>
         </is>
       </c>
       <c r="B5" s="4" t="inlineStr">
@@ -716,9 +716,9 @@
           <t>OFF</t>
         </is>
       </c>
-      <c r="C8" s="4" t="inlineStr">
-        <is>
-          <t>9:45AM-4PM</t>
+      <c r="C8" s="6" t="inlineStr">
+        <is>
+          <t>OFF</t>
         </is>
       </c>
       <c r="D8" s="6" t="inlineStr">
@@ -886,7 +886,7 @@
       </c>
       <c r="C12" s="4" t="inlineStr">
         <is>
-          <t>9:30AM-4PM</t>
+          <t>9:45AM-4PM</t>
         </is>
       </c>
       <c r="D12" s="6" t="inlineStr">
@@ -982,9 +982,9 @@
           <t>10AM-5PM</t>
         </is>
       </c>
-      <c r="C15" s="6" t="inlineStr">
-        <is>
-          <t>OFF</t>
+      <c r="C15" s="4" t="inlineStr">
+        <is>
+          <t>10AM-5PM</t>
         </is>
       </c>
       <c r="D15" s="4" t="inlineStr">
@@ -1024,9 +1024,9 @@
           <t>OFF</t>
         </is>
       </c>
-      <c r="C16" s="4" t="inlineStr">
-        <is>
-          <t>10AM-5PM</t>
+      <c r="C16" s="6" t="inlineStr">
+        <is>
+          <t>OFF</t>
         </is>
       </c>
       <c r="D16" s="6" t="inlineStr">
@@ -1323,130 +1323,136 @@
       </c>
       <c r="C27" s="7" t="inlineStr">
         <is>
+          <t>Lifeguard,
+9:30AM-4PM</t>
+        </is>
+      </c>
+      <c r="D27" s="7" t="inlineStr">
+        <is>
+          <t>Lifeguard,
+9:30AM-4PM</t>
+        </is>
+      </c>
+      <c r="E27" s="7" t="inlineStr">
+        <is>
+          <t>PA,
+10AM-5PM</t>
+        </is>
+      </c>
+      <c r="F27" s="7" t="inlineStr">
+        <is>
+          <t>Lifeguard,
+9:45AM-5PM</t>
+        </is>
+      </c>
+      <c r="G27" s="7" t="inlineStr">
+        <is>
+          <t>Lifeguard,
+9:45AM-5PM</t>
+        </is>
+      </c>
+      <c r="H27" s="7" t="inlineStr">
+        <is>
+          <t>Lifeguard,
+9:30AM-5PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" s="7" t="inlineStr">
+        <is>
+          <t>Lifeguard,
+9:30AM-4PM</t>
+        </is>
+      </c>
+      <c r="C28" s="7" t="inlineStr">
+        <is>
           <t>Bartender,
 10AM-4PM</t>
         </is>
       </c>
-      <c r="D27" s="7" t="inlineStr">
-        <is>
-          <t>Lifeguard,
-9:30AM-4PM</t>
-        </is>
-      </c>
-      <c r="E27" s="7" t="inlineStr">
+      <c r="E28" s="7" t="inlineStr">
+        <is>
+          <t>Consierge,
+9AM-5PM</t>
+        </is>
+      </c>
+      <c r="F28" s="7" t="inlineStr">
         <is>
           <t>PA,
 10AM-5PM</t>
         </is>
       </c>
-      <c r="F27" s="7" t="inlineStr">
+      <c r="G28" s="7" t="inlineStr">
         <is>
           <t>Lifeguard,
 9:45AM-5PM</t>
         </is>
       </c>
-      <c r="G27" s="7" t="inlineStr">
+      <c r="H28" s="7" t="inlineStr">
+        <is>
+          <t>PA,
+10AM-5PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" s="7" t="inlineStr">
+        <is>
+          <t>Bartender,
+10AM-4PM</t>
+        </is>
+      </c>
+      <c r="F29" s="7" t="inlineStr">
+        <is>
+          <t>Consierge,
+9AM-7PM</t>
+        </is>
+      </c>
+      <c r="G29" s="7" t="inlineStr">
         <is>
           <t>Lifeguard,
 9:45AM-5PM</t>
         </is>
       </c>
-      <c r="H27" s="7" t="inlineStr">
-        <is>
-          <t>Lifeguard,
-9:30AM-5PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" s="7" t="inlineStr">
-        <is>
-          <t>Lifeguard,
+      <c r="H29" s="7" t="inlineStr">
+        <is>
+          <t>Barback,
 9:30AM-4PM</t>
         </is>
       </c>
-      <c r="E28" s="7" t="inlineStr">
-        <is>
-          <t>Consierge,
-9AM-5PM</t>
-        </is>
-      </c>
-      <c r="F28" s="7" t="inlineStr">
+    </row>
+    <row r="30">
+      <c r="G30" s="7" t="inlineStr">
         <is>
           <t>PA,
 10AM-5PM</t>
         </is>
       </c>
-      <c r="G28" s="7" t="inlineStr">
-        <is>
-          <t>Lifeguard,
-9:45AM-5PM</t>
-        </is>
-      </c>
-      <c r="H28" s="7" t="inlineStr">
+    </row>
+    <row r="31">
+      <c r="G31" s="7" t="inlineStr">
         <is>
           <t>PA,
 10AM-5PM</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="B29" s="7" t="inlineStr">
-        <is>
-          <t>Bartender,
-10AM-4PM</t>
-        </is>
-      </c>
-      <c r="F29" s="7" t="inlineStr">
+    <row r="32">
+      <c r="G32" s="7" t="inlineStr">
         <is>
           <t>Consierge,
 9AM-7PM</t>
         </is>
       </c>
-      <c r="G29" s="7" t="inlineStr">
-        <is>
-          <t>Lifeguard,
-9:45AM-5PM</t>
-        </is>
-      </c>
-      <c r="H29" s="7" t="inlineStr">
-        <is>
-          <t>Barback,
-9:30AM-4PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="G30" s="7" t="inlineStr">
-        <is>
-          <t>PA,
-10AM-5PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="G31" s="7" t="inlineStr">
-        <is>
-          <t>PA,
-10AM-5PM</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="G32" s="7" t="inlineStr">
-        <is>
-          <t>Consierge,
-9AM-7PM</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A13:H13"/>
     <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A4:H4"/>
     <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A1:H1"/>
     <mergeCell ref="A23:H23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>